<commit_message>
update data and script
</commit_message>
<xml_diff>
--- a/data/history_vessel.xlsx
+++ b/data/history_vessel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="250">
   <si>
     <t>Vessel Name</t>
   </si>
@@ -49,6 +49,144 @@
     <t>Update Time</t>
   </si>
   <si>
+    <t>COSCO HOUSTON</t>
+  </si>
+  <si>
+    <t>TASMAN</t>
+  </si>
+  <si>
+    <t>EVER BOOMY</t>
+  </si>
+  <si>
+    <t>TANTO ALAM</t>
+  </si>
+  <si>
+    <t>URU BHUM</t>
+  </si>
+  <si>
+    <t>COSCO HAIFA</t>
+  </si>
+  <si>
+    <t>KMTC SHIMIZU</t>
+  </si>
+  <si>
+    <t>MERKUR FJORD</t>
+  </si>
+  <si>
+    <t>ZHONG GU PENG LAI</t>
+  </si>
+  <si>
+    <t>SPIL NINGSIH</t>
+  </si>
+  <si>
+    <t>MMSS 2503</t>
+  </si>
+  <si>
+    <t>AN HAI</t>
+  </si>
+  <si>
+    <t>MSC ANCONA III</t>
+  </si>
+  <si>
+    <t>TANTO BAGUS</t>
+  </si>
+  <si>
+    <t>WAN HAI 351</t>
+  </si>
+  <si>
+    <t>EVER CONFORM</t>
+  </si>
+  <si>
+    <t>ANTWERP BRIDGE</t>
+  </si>
+  <si>
+    <t>KAPPA</t>
+  </si>
+  <si>
+    <t>MSC ALDI III</t>
+  </si>
+  <si>
+    <t>WAN HAI 325</t>
+  </si>
+  <si>
+    <t>BELAWAN</t>
+  </si>
+  <si>
+    <t>TMS GLORY</t>
+  </si>
+  <si>
+    <t>SITC QIMING</t>
+  </si>
+  <si>
+    <t>LUMOSO GEMBIRA</t>
+  </si>
+  <si>
+    <t>SEASPAN KYOTO</t>
+  </si>
+  <si>
+    <t>XIN FANG CHENG</t>
+  </si>
+  <si>
+    <t>JML FORTUNE</t>
+  </si>
+  <si>
+    <t>BATANGHARI MAS</t>
+  </si>
+  <si>
+    <t>TIGER LONGKOU</t>
+  </si>
+  <si>
+    <t>KOKOPO CHIEF</t>
+  </si>
+  <si>
+    <t>INESSA</t>
+  </si>
+  <si>
+    <t>SCION MAFALDA</t>
+  </si>
+  <si>
+    <t>PULAU NUNUKAN</t>
+  </si>
+  <si>
+    <t>WAN HAI 371</t>
+  </si>
+  <si>
+    <t>MERATUS LEMBAR</t>
+  </si>
+  <si>
+    <t>MERATUS SABANG</t>
+  </si>
+  <si>
+    <t>SPIL RENATA</t>
+  </si>
+  <si>
+    <t>STARSHIP VENUS</t>
+  </si>
+  <si>
+    <t>FLORA DELMAS</t>
+  </si>
+  <si>
+    <t>TANTO KHARISMA</t>
+  </si>
+  <si>
+    <t>ZHONG GU TAI YUAN</t>
+  </si>
+  <si>
+    <t>WAN HAI 377</t>
+  </si>
+  <si>
+    <t>WAN HAI 509</t>
+  </si>
+  <si>
+    <t>BALI AYU</t>
+  </si>
+  <si>
+    <t>MSC ARIA III</t>
+  </si>
+  <si>
+    <t>TANTO TENANG</t>
+  </si>
+  <si>
     <t>APL PUSAN</t>
   </si>
   <si>
@@ -67,9 +205,6 @@
     <t>SITC SHENGMING</t>
   </si>
   <si>
-    <t>KMTC HAIPHONG</t>
-  </si>
-  <si>
     <t>EVER OBEY</t>
   </si>
   <si>
@@ -82,34 +217,67 @@
     <t>MERATUS LEMBATA</t>
   </si>
   <si>
-    <t>KMTC SHANGHAI</t>
-  </si>
-  <si>
     <t>SINAR SULAWESI</t>
   </si>
   <si>
     <t>TELUK BERAU</t>
   </si>
   <si>
-    <t>GIALOVA</t>
-  </si>
-  <si>
     <t>Jakarta, Indonesia</t>
   </si>
   <si>
     <t>Surabaya, Indonesia</t>
   </si>
   <si>
+    <t>Singapore, Singapore</t>
+  </si>
+  <si>
+    <t>Onsan, Korea</t>
+  </si>
+  <si>
+    <t>Dongguan Anch., China</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Nhava Sheva, India</t>
+  </si>
+  <si>
     <t>Semarang, Indonesia</t>
   </si>
   <si>
-    <t>Ho Chi Minh City, Vietnam</t>
+    <t>Singapore Anch. 4, Singapore</t>
+  </si>
+  <si>
+    <t>Hong Kong Anch., Hong Kong</t>
+  </si>
+  <si>
+    <t>Taboneo Anch., Indonesia</t>
   </si>
   <si>
     <t>Busan, Korea</t>
   </si>
   <si>
-    <t>Hong Kong, Hong Kong</t>
+    <t>IDDJT</t>
+  </si>
+  <si>
+    <t>ID SMG</t>
+  </si>
+  <si>
+    <t>SGSIG PEBGA</t>
+  </si>
+  <si>
+    <t>Makassar, Indonesia</t>
+  </si>
+  <si>
+    <t>Pasir Gudang, Johor, Malaysia</t>
+  </si>
+  <si>
+    <t>Dilli, East Timor</t>
+  </si>
+  <si>
+    <t>Madang, Papua New Guinea</t>
   </si>
   <si>
     <t>Port Klang, Malaysia</t>
@@ -130,6 +298,144 @@
     <t>Banjarmasin, Indonesia</t>
   </si>
   <si>
+    <t>03/02/2025 07:30</t>
+  </si>
+  <si>
+    <t>02/02/2025 14:30</t>
+  </si>
+  <si>
+    <t>03/02/2025 12:38</t>
+  </si>
+  <si>
+    <t>03/02/2025 21:10</t>
+  </si>
+  <si>
+    <t>13/02/2025 09:30</t>
+  </si>
+  <si>
+    <t>13/02/2025 07:00</t>
+  </si>
+  <si>
+    <t>14/02/2025 14:00</t>
+  </si>
+  <si>
+    <t>14/02/2025 15:00</t>
+  </si>
+  <si>
+    <t>02/02/2025 07:30</t>
+  </si>
+  <si>
+    <t>03/02/2025 01:55</t>
+  </si>
+  <si>
+    <t>03/02/2025 17:00</t>
+  </si>
+  <si>
+    <t>01/02/2025 16:00</t>
+  </si>
+  <si>
+    <t>01/02/2025 21:45</t>
+  </si>
+  <si>
+    <t>03/02/2025 01:02</t>
+  </si>
+  <si>
+    <t>10/02/2025 13:30</t>
+  </si>
+  <si>
+    <t>06/02/2025 22:00</t>
+  </si>
+  <si>
+    <t>01/02/2025 16:30</t>
+  </si>
+  <si>
+    <t>02/02/2025 00:27</t>
+  </si>
+  <si>
+    <t>03/02/2025 14:00</t>
+  </si>
+  <si>
+    <t>31/01/2025 20:25</t>
+  </si>
+  <si>
+    <t>01/02/2025 07:50</t>
+  </si>
+  <si>
+    <t>01/02/2025 14:25</t>
+  </si>
+  <si>
+    <t>01/02/2025 17:15</t>
+  </si>
+  <si>
+    <t>01/02/2025 23:40</t>
+  </si>
+  <si>
+    <t>29/01/2025 18:00</t>
+  </si>
+  <si>
+    <t>29/01/2025 20:20</t>
+  </si>
+  <si>
+    <t>31/01/2025 23:00</t>
+  </si>
+  <si>
+    <t>31/01/2025 23:30</t>
+  </si>
+  <si>
+    <t>31/01/2025 21:15</t>
+  </si>
+  <si>
+    <t>01/02/2025 06:50</t>
+  </si>
+  <si>
+    <t>31/01/2025 09:50</t>
+  </si>
+  <si>
+    <t>31/01/2025 13:30</t>
+  </si>
+  <si>
+    <t>31/01/2025 01:03</t>
+  </si>
+  <si>
+    <t>10/02/2025 14:00</t>
+  </si>
+  <si>
+    <t>28/01/2025 02:00</t>
+  </si>
+  <si>
+    <t>28/01/2025 14:00</t>
+  </si>
+  <si>
+    <t>30/01/2025 01:00</t>
+  </si>
+  <si>
+    <t>10/02/2025 22:00</t>
+  </si>
+  <si>
+    <t>30/01/2025 05:05</t>
+  </si>
+  <si>
+    <t>30/01/2025 12:20</t>
+  </si>
+  <si>
+    <t>24/01/2025 09:00</t>
+  </si>
+  <si>
+    <t>24/01/2025 23:00</t>
+  </si>
+  <si>
+    <t>24/01/2025 20:15</t>
+  </si>
+  <si>
+    <t>24/01/2025 14:43</t>
+  </si>
+  <si>
+    <t>24/01/2025 19:45</t>
+  </si>
+  <si>
+    <t>24/01/2025 23:30</t>
+  </si>
+  <si>
     <t>23/01/2025 08:00</t>
   </si>
   <si>
@@ -148,9 +454,6 @@
     <t>23/01/2025 18:08</t>
   </si>
   <si>
-    <t>03/02/2025 14:00</t>
-  </si>
-  <si>
     <t>24/01/2025 01:35</t>
   </si>
   <si>
@@ -163,9 +466,6 @@
     <t>23/01/2025 17:15</t>
   </si>
   <si>
-    <t>01/02/2025 18:00</t>
-  </si>
-  <si>
     <t>22/01/2025 08:50</t>
   </si>
   <si>
@@ -175,7 +475,127 @@
     <t>23/01/2025 11:05</t>
   </si>
   <si>
-    <t>01/02/2025 22:00</t>
+    <t>04/02/2025 10:00</t>
+  </si>
+  <si>
+    <t>04/02/2025 05:00</t>
+  </si>
+  <si>
+    <t>04/02/2025 09:00</t>
+  </si>
+  <si>
+    <t>14/02/2025 01:30</t>
+  </si>
+  <si>
+    <t>15/02/2025 10:00</t>
+  </si>
+  <si>
+    <t>16/02/2025 12:00</t>
+  </si>
+  <si>
+    <t>03/02/2025 22:00</t>
+  </si>
+  <si>
+    <t>03/02/2025 20:00</t>
+  </si>
+  <si>
+    <t>04/02/2025 02:00</t>
+  </si>
+  <si>
+    <t>03/02/2025 13:00</t>
+  </si>
+  <si>
+    <t>03/02/2025 09:00</t>
+  </si>
+  <si>
+    <t>03/02/2025 02:28</t>
+  </si>
+  <si>
+    <t>11/02/2025 12:30</t>
+  </si>
+  <si>
+    <t>07/02/2025 11:30</t>
+  </si>
+  <si>
+    <t>03/02/2025 04:00</t>
+  </si>
+  <si>
+    <t>02/02/2025 23:00</t>
+  </si>
+  <si>
+    <t>04/02/2025 08:30</t>
+  </si>
+  <si>
+    <t>02/02/2025 05:00</t>
+  </si>
+  <si>
+    <t>02/02/2025 20:30</t>
+  </si>
+  <si>
+    <t>02/02/2025 15:00</t>
+  </si>
+  <si>
+    <t>01/02/2025 09:00</t>
+  </si>
+  <si>
+    <t>01/02/2025 05:00</t>
+  </si>
+  <si>
+    <t>01/02/2025 06:30</t>
+  </si>
+  <si>
+    <t>01/02/2025 10:00</t>
+  </si>
+  <si>
+    <t>01/02/2025 13:00</t>
+  </si>
+  <si>
+    <t>01/02/2025 01:00</t>
+  </si>
+  <si>
+    <t>31/01/2025 20:00</t>
+  </si>
+  <si>
+    <t>31/01/2025 14:30</t>
+  </si>
+  <si>
+    <t>11/02/2025 15:00</t>
+  </si>
+  <si>
+    <t>28/01/2025 08:30</t>
+  </si>
+  <si>
+    <t>28/01/2025 00:00</t>
+  </si>
+  <si>
+    <t>30/01/2025 04:30</t>
+  </si>
+  <si>
+    <t>12/02/2025 07:00</t>
+  </si>
+  <si>
+    <t>30/01/2025 13:00</t>
+  </si>
+  <si>
+    <t>30/01/2025 14:00</t>
+  </si>
+  <si>
+    <t>25/01/2025 22:00</t>
+  </si>
+  <si>
+    <t>26/01/2025 01:00</t>
+  </si>
+  <si>
+    <t>26/01/2025 10:00</t>
+  </si>
+  <si>
+    <t>25/01/2025 01:00</t>
+  </si>
+  <si>
+    <t>25/01/2025 14:00</t>
+  </si>
+  <si>
+    <t>25/01/2025 02:00</t>
   </si>
   <si>
     <t>25/01/2025 00:00</t>
@@ -196,9 +616,6 @@
     <t>24/01/2025 16:30</t>
   </si>
   <si>
-    <t>04/02/2025 19:00</t>
-  </si>
-  <si>
     <t>24/01/2025 10:00</t>
   </si>
   <si>
@@ -211,9 +628,6 @@
     <t>24/01/2025 01:30</t>
   </si>
   <si>
-    <t>02/02/2025 15:00</t>
-  </si>
-  <si>
     <t>23/01/2025 21:00</t>
   </si>
   <si>
@@ -223,28 +637,118 @@
     <t>23/01/2025 17:00</t>
   </si>
   <si>
-    <t>03/02/2025 18:00</t>
+    <t>03/02/2025 23:00</t>
+  </si>
+  <si>
+    <t>12/02/2025 00:00</t>
+  </si>
+  <si>
+    <t>11/02/2025 00:00</t>
+  </si>
+  <si>
+    <t>13/02/2025 00:00</t>
+  </si>
+  <si>
+    <t>01/02/2025 15:30</t>
+  </si>
+  <si>
+    <t>03/02/2025 06:00</t>
+  </si>
+  <si>
+    <t>02/02/2025 11:00</t>
+  </si>
+  <si>
+    <t>03/02/2025 00:00</t>
+  </si>
+  <si>
+    <t>02/02/2025 20:00</t>
+  </si>
+  <si>
+    <t>02/02/2025 13:00</t>
+  </si>
+  <si>
+    <t>01/02/2025 20:00</t>
+  </si>
+  <si>
+    <t>30/01/2025 18:00</t>
+  </si>
+  <si>
+    <t>30/01/2025 13:59</t>
+  </si>
+  <si>
+    <t>29/01/2025 21:00</t>
+  </si>
+  <si>
+    <t>01/01/2025 17:00</t>
+  </si>
+  <si>
+    <t>30/01/2025 22:00</t>
+  </si>
+  <si>
+    <t>25/01/2025 06:00</t>
+  </si>
+  <si>
+    <t>28/01/2025 18:00</t>
+  </si>
+  <si>
+    <t>29/01/2025 19:00</t>
+  </si>
+  <si>
+    <t>09/02/2025 00:00</t>
+  </si>
+  <si>
+    <t>29/01/2025 22:00</t>
+  </si>
+  <si>
+    <t>22/01/2025 21:00</t>
+  </si>
+  <si>
+    <t>24/01/2025 16:45</t>
+  </si>
+  <si>
+    <t>25/01/2025 01:55</t>
+  </si>
+  <si>
+    <t>19/01/2025 00:00</t>
   </si>
   <si>
     <t>18/01/2025 11:30</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>22/01/2025 13:30</t>
   </si>
   <si>
-    <t>02/01/2025 00:00</t>
-  </si>
-  <si>
     <t>20/01/2025 17:00</t>
   </si>
   <si>
-    <t>26/01/2025 00:00</t>
-  </si>
-  <si>
-    <t>28/01/2025 00:00</t>
+    <t>28/01/2025 01:00</t>
+  </si>
+  <si>
+    <t>29/01/2025 01:00</t>
+  </si>
+  <si>
+    <t>28/01/2025 20:00</t>
+  </si>
+  <si>
+    <t>27/01/2025 01:00</t>
+  </si>
+  <si>
+    <t>18/01/2025 12:00</t>
+  </si>
+  <si>
+    <t>22/01/2025 18:00</t>
+  </si>
+  <si>
+    <t>23/01/2025 01:00</t>
+  </si>
+  <si>
+    <t>18/01/2025 01:00</t>
+  </si>
+  <si>
+    <t>20/01/2025 01:00</t>
+  </si>
+  <si>
+    <t>21/01/2025 01:00</t>
   </si>
   <si>
     <t>13/01/2025 01:00</t>
@@ -621,7 +1125,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -667,34 +1171,34 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>9234123</v>
+        <v>9484273</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="E2" s="2">
-        <v>45680.04166666666</v>
+        <v>45690.16666666666</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>153</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>207</v>
       </c>
       <c r="I2" t="s">
-        <v>77</v>
+        <v>235</v>
       </c>
       <c r="J2" t="s">
-        <v>80</v>
+        <v>248</v>
       </c>
       <c r="K2" s="2">
-        <v>45682.04166666666</v>
+        <v>45692.47013888889</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -702,34 +1206,34 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>9786968</v>
+        <v>9189342</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="E3" s="2">
-        <v>45680.96180555555</v>
+        <v>45690.60416666666</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>154</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J3" t="s">
-        <v>80</v>
+        <v>248</v>
       </c>
       <c r="K3" s="2">
-        <v>45681.91666666666</v>
+        <v>45692.47013888889</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -737,34 +1241,34 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <v>9153410</v>
+        <v>9787015</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="E4" s="2">
-        <v>45679.625</v>
+        <v>45691.52638888889</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>155</v>
       </c>
       <c r="H4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J4" t="s">
-        <v>80</v>
+        <v>248</v>
       </c>
       <c r="K4" s="2">
-        <v>45681.79583333333</v>
+        <v>45692.47013888889</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -772,34 +1276,34 @@
         <v>14</v>
       </c>
       <c r="B5">
-        <v>9871440</v>
+        <v>9085699</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="E5" s="2">
-        <v>45681.48263888889</v>
+        <v>45691.88194444445</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>154</v>
       </c>
       <c r="H5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J5" t="s">
-        <v>80</v>
+        <v>248</v>
       </c>
       <c r="K5" s="2">
-        <v>45681.79513888889</v>
+        <v>45692.47013888889</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -807,34 +1311,34 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <v>9315343</v>
+        <v>9293234</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="E6" s="2">
-        <v>45680.52777777778</v>
+        <v>45701.25</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="G6" t="s">
-        <v>58</v>
+        <v>156</v>
       </c>
       <c r="H6" t="s">
-        <v>71</v>
+        <v>208</v>
       </c>
       <c r="I6" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J6" t="s">
-        <v>80</v>
+        <v>249</v>
       </c>
       <c r="K6" s="2">
-        <v>45681.70972222222</v>
+        <v>45692.47013888889</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -842,34 +1346,34 @@
         <v>16</v>
       </c>
       <c r="B7">
-        <v>9941063</v>
+        <v>9484338</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="E7" s="2">
-        <v>45680.75555555556</v>
+        <v>45701.25</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="H7" t="s">
-        <v>71</v>
+        <v>209</v>
       </c>
       <c r="I7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J7" t="s">
-        <v>80</v>
+        <v>249</v>
       </c>
       <c r="K7" s="2">
-        <v>45681.62986111111</v>
+        <v>45692.47013888889</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -877,34 +1381,34 @@
         <v>17</v>
       </c>
       <c r="B8">
-        <v>9793806</v>
+        <v>9893591</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="E8" s="2">
-        <v>45691.5</v>
+        <v>45702.54166666666</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>60</v>
+        <v>157</v>
       </c>
       <c r="H8" t="s">
-        <v>73</v>
+        <v>209</v>
       </c>
       <c r="I8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J8" t="s">
-        <v>81</v>
+        <v>249</v>
       </c>
       <c r="K8" s="2">
-        <v>45681.39513888889</v>
+        <v>45692.47013888889</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -912,34 +1416,34 @@
         <v>18</v>
       </c>
       <c r="B9">
-        <v>9919462</v>
+        <v>9620607</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="E9" s="2">
-        <v>45681.06597222222</v>
+        <v>45702.58333333334</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>158</v>
       </c>
       <c r="H9" t="s">
-        <v>71</v>
+        <v>210</v>
       </c>
       <c r="I9" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J9" t="s">
-        <v>80</v>
+        <v>249</v>
       </c>
       <c r="K9" s="2">
-        <v>45681.39444444444</v>
+        <v>45692.47013888889</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -947,34 +1451,34 @@
         <v>19</v>
       </c>
       <c r="B10">
-        <v>9463279</v>
+        <v>9809203</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="E10" s="2">
-        <v>45678.58333333334</v>
+        <v>45690.20833333334</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>159</v>
       </c>
       <c r="H10" t="s">
-        <v>74</v>
+        <v>211</v>
       </c>
       <c r="I10" t="s">
-        <v>79</v>
+        <v>236</v>
       </c>
       <c r="J10" t="s">
-        <v>80</v>
+        <v>248</v>
       </c>
       <c r="K10" s="2">
-        <v>45680.95902777778</v>
+        <v>45691.67083333333</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -982,34 +1486,34 @@
         <v>20</v>
       </c>
       <c r="B11">
-        <v>525015391</v>
+        <v>9273959</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="E11" s="2">
-        <v>45680.56319444445</v>
+        <v>45691.07986111111</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>160</v>
       </c>
       <c r="H11" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I11" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J11" t="s">
-        <v>80</v>
+        <v>248</v>
       </c>
       <c r="K11" s="2">
-        <v>45680.95833333334</v>
+        <v>45691.67083333333</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1017,34 +1521,34 @@
         <v>21</v>
       </c>
       <c r="B12">
-        <v>9821536</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="E12" s="2">
-        <v>45680.71875</v>
+        <v>45691.66666666666</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>161</v>
       </c>
       <c r="H12" t="s">
-        <v>71</v>
+        <v>212</v>
       </c>
       <c r="I12" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J12" t="s">
-        <v>80</v>
+        <v>249</v>
       </c>
       <c r="K12" s="2">
-        <v>45680.95833333334</v>
+        <v>45691.67083333333</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1052,34 +1556,34 @@
         <v>22</v>
       </c>
       <c r="B13">
-        <v>9274202</v>
+        <v>9238155</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="E13" s="2">
-        <v>45689.70833333334</v>
+        <v>45689.5</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>162</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>213</v>
       </c>
       <c r="I13" t="s">
-        <v>71</v>
+        <v>236</v>
       </c>
       <c r="J13" t="s">
-        <v>81</v>
+        <v>248</v>
       </c>
       <c r="K13" s="2">
-        <v>45680.95902777778</v>
+        <v>45691.58402777778</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1087,139 +1591,1641 @@
         <v>23</v>
       </c>
       <c r="B14">
-        <v>1015363</v>
+        <v>9259379</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="E14" s="2">
-        <v>45679.36805555555</v>
+        <v>45689.90625</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="G14" t="s">
-        <v>66</v>
+        <v>163</v>
       </c>
       <c r="H14" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I14" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J14" t="s">
-        <v>80</v>
+        <v>248</v>
       </c>
       <c r="K14" s="2">
-        <v>45680.83472222222</v>
+        <v>45691.58402777778</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B15">
-        <v>9871440</v>
+        <v>9210725</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="E15" s="2">
-        <v>45680.53125</v>
+        <v>45691.04305555556</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
       <c r="G15" t="s">
-        <v>67</v>
+        <v>164</v>
       </c>
       <c r="H15" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I15" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J15" t="s">
-        <v>80</v>
+        <v>248</v>
       </c>
       <c r="K15" s="2">
-        <v>45680.83472222222</v>
+        <v>45691.58402777778</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16">
-        <v>9563976</v>
+        <v>9553763</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="E16" s="2">
-        <v>45680.46180555555</v>
+        <v>45698.52083333334</v>
       </c>
       <c r="F16" t="s">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="G16" t="s">
-        <v>68</v>
+        <v>165</v>
       </c>
       <c r="H16" t="s">
-        <v>71</v>
+        <v>214</v>
       </c>
       <c r="I16" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J16" t="s">
-        <v>80</v>
+        <v>249</v>
       </c>
       <c r="K16" s="2">
-        <v>45680.66736111111</v>
+        <v>45691.58402777778</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17">
-        <v>9400306</v>
+        <v>9913846</v>
       </c>
       <c r="C17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="2">
+        <v>45694.91666666666</v>
+      </c>
+      <c r="F17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" t="s">
+        <v>166</v>
+      </c>
+      <c r="H17" t="s">
+        <v>215</v>
+      </c>
+      <c r="I17" t="s">
+        <v>237</v>
+      </c>
+      <c r="J17" t="s">
+        <v>249</v>
+      </c>
+      <c r="K17" s="2">
+        <v>45691.58402777778</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>9297527</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="2">
+        <v>45689.45833333334</v>
+      </c>
+      <c r="F18" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" t="s">
+        <v>167</v>
+      </c>
+      <c r="H18" t="s">
+        <v>216</v>
+      </c>
+      <c r="I18" t="s">
+        <v>235</v>
+      </c>
+      <c r="J18" t="s">
+        <v>248</v>
+      </c>
+      <c r="K18" s="2">
+        <v>45691.08680555555</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>9532745</v>
+      </c>
+      <c r="C19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="2">
+        <v>45690.01875</v>
+      </c>
+      <c r="F19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G19" t="s">
+        <v>168</v>
+      </c>
+      <c r="H19" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19" t="s">
+        <v>74</v>
+      </c>
+      <c r="J19" t="s">
+        <v>248</v>
+      </c>
+      <c r="K19" s="2">
+        <v>45691.08680555555</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>9341122</v>
+      </c>
+      <c r="C20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="2">
+        <v>45691.58333333334</v>
+      </c>
+      <c r="F20" t="s">
+        <v>112</v>
+      </c>
+      <c r="G20" t="s">
+        <v>169</v>
+      </c>
+      <c r="H20" t="s">
+        <v>217</v>
+      </c>
+      <c r="I20" t="s">
+        <v>128</v>
+      </c>
+      <c r="J20" t="s">
+        <v>249</v>
+      </c>
+      <c r="K20" s="2">
+        <v>45691.08680555555</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>9871476</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="2">
+        <v>45688.85069444445</v>
+      </c>
+      <c r="F21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G21" t="s">
+        <v>170</v>
+      </c>
+      <c r="H21" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" t="s">
+        <v>74</v>
+      </c>
+      <c r="J21" t="s">
+        <v>248</v>
+      </c>
+      <c r="K21" s="2">
+        <v>45690.83858877315</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
         <v>31</v>
       </c>
-      <c r="D17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="2">
-        <v>45689.20833333334</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="B22">
+        <v>9412828</v>
+      </c>
+      <c r="C22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="2">
+        <v>45689.32638888889</v>
+      </c>
+      <c r="F22" t="s">
+        <v>114</v>
+      </c>
+      <c r="G22" t="s">
+        <v>171</v>
+      </c>
+      <c r="H22" t="s">
+        <v>74</v>
+      </c>
+      <c r="I22" t="s">
+        <v>74</v>
+      </c>
+      <c r="J22" t="s">
+        <v>248</v>
+      </c>
+      <c r="K22" s="2">
+        <v>45691.83858877315</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>9065431</v>
+      </c>
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="2">
+        <v>45689.45833333334</v>
+      </c>
+      <c r="F23" t="s">
+        <v>115</v>
+      </c>
+      <c r="G23" t="s">
+        <v>170</v>
+      </c>
+      <c r="H23" t="s">
+        <v>218</v>
+      </c>
+      <c r="I23" t="s">
+        <v>74</v>
+      </c>
+      <c r="J23" t="s">
+        <v>248</v>
+      </c>
+      <c r="K23" s="2">
+        <v>45692.83858877315</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24">
+        <v>9932878</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="2">
+        <v>45689.71875</v>
+      </c>
+      <c r="F24" t="s">
+        <v>116</v>
+      </c>
+      <c r="G24" t="s">
+        <v>170</v>
+      </c>
+      <c r="H24" t="s">
+        <v>74</v>
+      </c>
+      <c r="I24" t="s">
+        <v>74</v>
+      </c>
+      <c r="J24" t="s">
+        <v>248</v>
+      </c>
+      <c r="K24" s="2">
+        <v>45695.83858877315</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>9491654</v>
+      </c>
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="2">
+        <v>45689.98611111111</v>
+      </c>
+      <c r="F25" t="s">
+        <v>117</v>
+      </c>
+      <c r="G25" t="s">
+        <v>172</v>
+      </c>
+      <c r="H25" t="s">
+        <v>74</v>
+      </c>
+      <c r="I25" t="s">
+        <v>74</v>
+      </c>
+      <c r="J25" t="s">
+        <v>248</v>
+      </c>
+      <c r="K25" s="2">
+        <v>45697.83858877315</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>9492696</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="2">
+        <v>45686.41666666666</v>
+      </c>
+      <c r="F26" t="s">
+        <v>118</v>
+      </c>
+      <c r="G26" t="s">
+        <v>173</v>
+      </c>
+      <c r="H26" t="s">
+        <v>219</v>
+      </c>
+      <c r="I26" t="s">
+        <v>191</v>
+      </c>
+      <c r="J26" t="s">
+        <v>248</v>
+      </c>
+      <c r="K26" s="2">
+        <v>45689.25347222222</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <v>9309930</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="2">
+        <v>45686.75</v>
+      </c>
+      <c r="F27" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" t="s">
+        <v>174</v>
+      </c>
+      <c r="H27" t="s">
+        <v>220</v>
+      </c>
+      <c r="I27" t="s">
+        <v>238</v>
+      </c>
+      <c r="J27" t="s">
+        <v>248</v>
+      </c>
+      <c r="K27" s="2">
+        <v>45689.25347222222</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28">
+        <v>8598132</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="2">
+        <v>45688.625</v>
+      </c>
+      <c r="F28" t="s">
+        <v>120</v>
+      </c>
+      <c r="G28" t="s">
+        <v>173</v>
+      </c>
+      <c r="H28" t="s">
+        <v>221</v>
+      </c>
+      <c r="I28" t="s">
+        <v>74</v>
+      </c>
+      <c r="J28" t="s">
+        <v>248</v>
+      </c>
+      <c r="K28" s="2">
+        <v>45689.17569444444</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29">
+        <v>9586291</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="2">
+        <v>45688.79166666666</v>
+      </c>
+      <c r="F29" t="s">
+        <v>121</v>
+      </c>
+      <c r="G29" t="s">
+        <v>175</v>
+      </c>
+      <c r="H29" t="s">
+        <v>222</v>
+      </c>
+      <c r="I29" t="s">
+        <v>74</v>
+      </c>
+      <c r="J29" t="s">
+        <v>248</v>
+      </c>
+      <c r="K29" s="2">
+        <v>45689.25347222222</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <v>9913547</v>
+      </c>
+      <c r="C30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="2">
+        <v>45688.88541666666</v>
+      </c>
+      <c r="F30" t="s">
+        <v>122</v>
+      </c>
+      <c r="G30" t="s">
+        <v>176</v>
+      </c>
+      <c r="H30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I30" t="s">
+        <v>74</v>
+      </c>
+      <c r="J30" t="s">
+        <v>248</v>
+      </c>
+      <c r="K30" s="2">
+        <v>45689.50138888889</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <v>8907412</v>
+      </c>
+      <c r="C31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="2">
+        <v>45689.28472222222</v>
+      </c>
+      <c r="F31" t="s">
+        <v>123</v>
+      </c>
+      <c r="G31" t="s">
+        <v>177</v>
+      </c>
+      <c r="H31" t="s">
+        <v>74</v>
+      </c>
+      <c r="I31" t="s">
+        <v>74</v>
+      </c>
+      <c r="J31" t="s">
+        <v>248</v>
+      </c>
+      <c r="K31" s="2">
+        <v>45689.58888888889</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <v>9832999</v>
+      </c>
+      <c r="C32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="2">
+        <v>45688.40972222222</v>
+      </c>
+      <c r="F32" t="s">
+        <v>124</v>
+      </c>
+      <c r="G32" t="s">
+        <v>178</v>
+      </c>
+      <c r="H32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I32" t="s">
+        <v>74</v>
+      </c>
+      <c r="J32" t="s">
+        <v>248</v>
+      </c>
+      <c r="K32" s="2">
+        <v>45689.00138888889</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33">
+        <v>9675810</v>
+      </c>
+      <c r="C33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="2">
+        <v>45688.5625</v>
+      </c>
+      <c r="F33" t="s">
+        <v>125</v>
+      </c>
+      <c r="G33" t="s">
+        <v>179</v>
+      </c>
+      <c r="H33" t="s">
+        <v>74</v>
+      </c>
+      <c r="I33" t="s">
+        <v>74</v>
+      </c>
+      <c r="J33" t="s">
+        <v>248</v>
+      </c>
+      <c r="K33" s="2">
+        <v>45688.8875</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34">
+        <v>9649598</v>
+      </c>
+      <c r="C34" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="2">
+        <v>45688.04375</v>
+      </c>
+      <c r="F34" t="s">
+        <v>126</v>
+      </c>
+      <c r="G34" t="s">
+        <v>180</v>
+      </c>
+      <c r="H34" t="s">
+        <v>74</v>
+      </c>
+      <c r="I34" t="s">
+        <v>74</v>
+      </c>
+      <c r="J34" t="s">
+        <v>248</v>
+      </c>
+      <c r="K34" s="2">
+        <v>45688.67083333333</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35">
+        <v>9958107</v>
+      </c>
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" s="2">
+        <v>45698.5</v>
+      </c>
+      <c r="F35" t="s">
+        <v>127</v>
+      </c>
+      <c r="G35" t="s">
+        <v>181</v>
+      </c>
+      <c r="H35" t="s">
+        <v>214</v>
+      </c>
+      <c r="I35" t="s">
+        <v>74</v>
+      </c>
+      <c r="J35" t="s">
+        <v>249</v>
+      </c>
+      <c r="K35" s="2">
+        <v>45688.67083333333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36">
+        <v>9821524</v>
+      </c>
+      <c r="C36" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="2">
+        <v>45685.08333333334</v>
+      </c>
+      <c r="F36" t="s">
+        <v>128</v>
+      </c>
+      <c r="G36" t="s">
+        <v>182</v>
+      </c>
+      <c r="H36" t="s">
+        <v>223</v>
+      </c>
+      <c r="I36" t="s">
+        <v>239</v>
+      </c>
+      <c r="J36" t="s">
+        <v>249</v>
+      </c>
+      <c r="K36" s="2">
+        <v>45688.57361111111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37">
+        <v>9018311</v>
+      </c>
+      <c r="C37" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" t="s">
+        <v>76</v>
+      </c>
+      <c r="E37" s="2">
+        <v>45685.58333333334</v>
+      </c>
+      <c r="F37" t="s">
+        <v>129</v>
+      </c>
+      <c r="G37" t="s">
+        <v>183</v>
+      </c>
+      <c r="H37" t="s">
+        <v>224</v>
+      </c>
+      <c r="I37" t="s">
+        <v>240</v>
+      </c>
+      <c r="J37" t="s">
+        <v>249</v>
+      </c>
+      <c r="K37" s="2">
+        <v>45688.57361111111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38">
+        <v>9834533</v>
+      </c>
+      <c r="C38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" t="s">
+        <v>76</v>
+      </c>
+      <c r="E38" s="2">
+        <v>45687.04166666666</v>
+      </c>
+      <c r="F38" t="s">
+        <v>130</v>
+      </c>
+      <c r="G38" t="s">
+        <v>184</v>
+      </c>
+      <c r="H38" t="s">
+        <v>225</v>
+      </c>
+      <c r="I38" t="s">
+        <v>241</v>
+      </c>
+      <c r="J38" t="s">
+        <v>249</v>
+      </c>
+      <c r="K38" s="2">
+        <v>45688.57361111111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39">
+        <v>9981116</v>
+      </c>
+      <c r="C39" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="2">
+        <v>45698.875</v>
+      </c>
+      <c r="F39" t="s">
+        <v>131</v>
+      </c>
+      <c r="G39" t="s">
+        <v>185</v>
+      </c>
+      <c r="H39" t="s">
+        <v>226</v>
+      </c>
+      <c r="I39" t="s">
+        <v>74</v>
+      </c>
+      <c r="J39" t="s">
+        <v>249</v>
+      </c>
+      <c r="K39" s="2">
+        <v>45688.57361111111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40">
+        <v>9239862</v>
+      </c>
+      <c r="C40" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" s="2">
+        <v>45687.21180555555</v>
+      </c>
+      <c r="F40" t="s">
+        <v>132</v>
+      </c>
+      <c r="G40" t="s">
+        <v>186</v>
+      </c>
+      <c r="H40" t="s">
+        <v>74</v>
+      </c>
+      <c r="I40" t="s">
+        <v>74</v>
+      </c>
+      <c r="J40" t="s">
+        <v>248</v>
+      </c>
+      <c r="K40" s="2">
+        <v>45687.63888888889</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41">
+        <v>9915387</v>
+      </c>
+      <c r="C41" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="2">
+        <v>45687.33333333334</v>
+      </c>
+      <c r="F41" t="s">
+        <v>133</v>
+      </c>
+      <c r="G41" t="s">
+        <v>187</v>
+      </c>
+      <c r="H41" t="s">
+        <v>227</v>
+      </c>
+      <c r="I41" t="s">
+        <v>74</v>
+      </c>
+      <c r="J41" t="s">
+        <v>248</v>
+      </c>
+      <c r="K41" s="2">
+        <v>45687.63888888889</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42">
+        <v>9933860</v>
+      </c>
+      <c r="C42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" t="s">
+        <v>69</v>
+      </c>
+      <c r="E42" s="2">
+        <v>45680.79166666666</v>
+      </c>
+      <c r="F42" t="s">
+        <v>134</v>
+      </c>
+      <c r="G42" t="s">
+        <v>188</v>
+      </c>
+      <c r="H42" t="s">
+        <v>228</v>
+      </c>
+      <c r="I42" t="s">
+        <v>242</v>
+      </c>
+      <c r="J42" t="s">
+        <v>248</v>
+      </c>
+      <c r="K42" s="2">
+        <v>45682.08402777778</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43">
+        <v>9958133</v>
+      </c>
+      <c r="C43" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E43" s="2">
+        <v>45680.95833333334</v>
+      </c>
+      <c r="F43" t="s">
+        <v>135</v>
+      </c>
+      <c r="G43" t="s">
+        <v>189</v>
+      </c>
+      <c r="H43" t="s">
+        <v>229</v>
+      </c>
+      <c r="I43" t="s">
+        <v>243</v>
+      </c>
+      <c r="J43" t="s">
+        <v>248</v>
+      </c>
+      <c r="K43" s="2">
+        <v>45682.08402777778</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" t="s">
         <v>53</v>
       </c>
-      <c r="G17" t="s">
-        <v>69</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="B44">
+        <v>9326421</v>
+      </c>
+      <c r="C44" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" t="s">
+        <v>71</v>
+      </c>
+      <c r="E44" s="2">
+        <v>45681.5</v>
+      </c>
+      <c r="F44" t="s">
+        <v>136</v>
+      </c>
+      <c r="G44" t="s">
+        <v>190</v>
+      </c>
+      <c r="H44" t="s">
+        <v>230</v>
+      </c>
+      <c r="I44" t="s">
+        <v>244</v>
+      </c>
+      <c r="J44" t="s">
+        <v>248</v>
+      </c>
+      <c r="K44" s="2">
+        <v>45682.08402777778</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45">
+        <v>9393046</v>
+      </c>
+      <c r="C45" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" t="s">
+        <v>70</v>
+      </c>
+      <c r="E45" s="2">
+        <v>45681.61319444444</v>
+      </c>
+      <c r="F45" t="s">
+        <v>137</v>
+      </c>
+      <c r="G45" t="s">
+        <v>191</v>
+      </c>
+      <c r="H45" t="s">
+        <v>74</v>
+      </c>
+      <c r="I45" t="s">
+        <v>74</v>
+      </c>
+      <c r="J45" t="s">
+        <v>248</v>
+      </c>
+      <c r="K45" s="2">
+        <v>45682.08333333334</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46">
+        <v>9374595</v>
+      </c>
+      <c r="C46" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" t="s">
+        <v>70</v>
+      </c>
+      <c r="E46" s="2">
+        <v>45681.82291666666</v>
+      </c>
+      <c r="F46" t="s">
+        <v>138</v>
+      </c>
+      <c r="G46" t="s">
+        <v>192</v>
+      </c>
+      <c r="H46" t="s">
+        <v>74</v>
+      </c>
+      <c r="I46" t="s">
+        <v>74</v>
+      </c>
+      <c r="J46" t="s">
+        <v>248</v>
+      </c>
+      <c r="K46" s="2">
+        <v>45682.08333333334</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47">
+        <v>9192040</v>
+      </c>
+      <c r="C47" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" t="s">
+        <v>69</v>
+      </c>
+      <c r="E47" s="2">
+        <v>45681.875</v>
+      </c>
+      <c r="F47" t="s">
+        <v>139</v>
+      </c>
+      <c r="G47" t="s">
+        <v>193</v>
+      </c>
+      <c r="H47" t="s">
+        <v>231</v>
+      </c>
+      <c r="I47" t="s">
+        <v>74</v>
+      </c>
+      <c r="J47" t="s">
+        <v>248</v>
+      </c>
+      <c r="K47" s="2">
+        <v>45682.08402777778</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48">
+        <v>9234123</v>
+      </c>
+      <c r="C48" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" s="2">
+        <v>45680.04166666666</v>
+      </c>
+      <c r="F48" t="s">
+        <v>140</v>
+      </c>
+      <c r="G48" t="s">
+        <v>194</v>
+      </c>
+      <c r="H48" t="s">
+        <v>232</v>
+      </c>
+      <c r="I48" t="s">
+        <v>245</v>
+      </c>
+      <c r="J48" t="s">
+        <v>248</v>
+      </c>
+      <c r="K48" s="2">
+        <v>45682.04166666666</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49">
+        <v>9786968</v>
+      </c>
+      <c r="C49" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" t="s">
+        <v>89</v>
+      </c>
+      <c r="E49" s="2">
+        <v>45680.96180555555</v>
+      </c>
+      <c r="F49" t="s">
+        <v>141</v>
+      </c>
+      <c r="G49" t="s">
+        <v>195</v>
+      </c>
+      <c r="H49" t="s">
+        <v>74</v>
+      </c>
+      <c r="I49" t="s">
+        <v>74</v>
+      </c>
+      <c r="J49" t="s">
+        <v>248</v>
+      </c>
+      <c r="K49" s="2">
+        <v>45681.91666666666</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50">
+        <v>9153410</v>
+      </c>
+      <c r="C50" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50" t="s">
+        <v>70</v>
+      </c>
+      <c r="E50" s="2">
+        <v>45679.625</v>
+      </c>
+      <c r="F50" t="s">
+        <v>142</v>
+      </c>
+      <c r="G50" t="s">
+        <v>196</v>
+      </c>
+      <c r="H50" t="s">
+        <v>233</v>
+      </c>
+      <c r="I50" t="s">
+        <v>246</v>
+      </c>
+      <c r="J50" t="s">
+        <v>248</v>
+      </c>
+      <c r="K50" s="2">
+        <v>45681.79583333333</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51">
+        <v>9871440</v>
+      </c>
+      <c r="C51" t="s">
+        <v>70</v>
+      </c>
+      <c r="D51" t="s">
+        <v>90</v>
+      </c>
+      <c r="E51" s="2">
+        <v>45681.48263888889</v>
+      </c>
+      <c r="F51" t="s">
+        <v>143</v>
+      </c>
+      <c r="G51" t="s">
+        <v>197</v>
+      </c>
+      <c r="H51" t="s">
+        <v>74</v>
+      </c>
+      <c r="I51" t="s">
+        <v>74</v>
+      </c>
+      <c r="J51" t="s">
+        <v>248</v>
+      </c>
+      <c r="K51" s="2">
+        <v>45681.79513888889</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52">
+        <v>9315343</v>
+      </c>
+      <c r="C52" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" t="s">
+        <v>69</v>
+      </c>
+      <c r="E52" s="2">
+        <v>45680.52777777778</v>
+      </c>
+      <c r="F52" t="s">
+        <v>144</v>
+      </c>
+      <c r="G52" t="s">
+        <v>198</v>
+      </c>
+      <c r="H52" t="s">
+        <v>74</v>
+      </c>
+      <c r="I52" t="s">
+        <v>74</v>
+      </c>
+      <c r="J52" t="s">
+        <v>248</v>
+      </c>
+      <c r="K52" s="2">
+        <v>45681.70972222222</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53">
+        <v>9941063</v>
+      </c>
+      <c r="C53" t="s">
         <v>76</v>
       </c>
-      <c r="I17" t="s">
-        <v>71</v>
-      </c>
-      <c r="J17" t="s">
-        <v>81</v>
-      </c>
-      <c r="K17" s="2">
-        <v>45680.64513888889</v>
+      <c r="D53" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53" s="2">
+        <v>45680.75555555556</v>
+      </c>
+      <c r="F53" t="s">
+        <v>145</v>
+      </c>
+      <c r="G53" t="s">
+        <v>199</v>
+      </c>
+      <c r="H53" t="s">
+        <v>74</v>
+      </c>
+      <c r="I53" t="s">
+        <v>74</v>
+      </c>
+      <c r="J53" t="s">
+        <v>248</v>
+      </c>
+      <c r="K53" s="2">
+        <v>45681.62986111111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54">
+        <v>9919462</v>
+      </c>
+      <c r="C54" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54" t="s">
+        <v>70</v>
+      </c>
+      <c r="E54" s="2">
+        <v>45681.06597222222</v>
+      </c>
+      <c r="F54" t="s">
+        <v>146</v>
+      </c>
+      <c r="G54" t="s">
+        <v>200</v>
+      </c>
+      <c r="H54" t="s">
+        <v>74</v>
+      </c>
+      <c r="I54" t="s">
+        <v>74</v>
+      </c>
+      <c r="J54" t="s">
+        <v>248</v>
+      </c>
+      <c r="K54" s="2">
+        <v>45681.39444444444</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55">
+        <v>9463279</v>
+      </c>
+      <c r="C55" t="s">
+        <v>69</v>
+      </c>
+      <c r="D55" t="s">
+        <v>69</v>
+      </c>
+      <c r="E55" s="2">
+        <v>45678.58333333334</v>
+      </c>
+      <c r="F55" t="s">
+        <v>147</v>
+      </c>
+      <c r="G55" t="s">
+        <v>201</v>
+      </c>
+      <c r="H55" t="s">
+        <v>234</v>
+      </c>
+      <c r="I55" t="s">
+        <v>247</v>
+      </c>
+      <c r="J55" t="s">
+        <v>248</v>
+      </c>
+      <c r="K55" s="2">
+        <v>45680.95902777778</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56">
+        <v>525015391</v>
+      </c>
+      <c r="C56" t="s">
+        <v>76</v>
+      </c>
+      <c r="D56" t="s">
+        <v>69</v>
+      </c>
+      <c r="E56" s="2">
+        <v>45680.56319444445</v>
+      </c>
+      <c r="F56" t="s">
+        <v>148</v>
+      </c>
+      <c r="G56" t="s">
+        <v>202</v>
+      </c>
+      <c r="H56" t="s">
+        <v>74</v>
+      </c>
+      <c r="I56" t="s">
+        <v>74</v>
+      </c>
+      <c r="J56" t="s">
+        <v>248</v>
+      </c>
+      <c r="K56" s="2">
+        <v>45680.95833333334</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57">
+        <v>9821536</v>
+      </c>
+      <c r="C57" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" t="s">
+        <v>70</v>
+      </c>
+      <c r="E57" s="2">
+        <v>45680.71875</v>
+      </c>
+      <c r="F57" t="s">
+        <v>149</v>
+      </c>
+      <c r="G57" t="s">
+        <v>203</v>
+      </c>
+      <c r="H57" t="s">
+        <v>74</v>
+      </c>
+      <c r="I57" t="s">
+        <v>74</v>
+      </c>
+      <c r="J57" t="s">
+        <v>248</v>
+      </c>
+      <c r="K57" s="2">
+        <v>45680.95833333334</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58">
+        <v>1015363</v>
+      </c>
+      <c r="C58" t="s">
+        <v>70</v>
+      </c>
+      <c r="D58" t="s">
+        <v>91</v>
+      </c>
+      <c r="E58" s="2">
+        <v>45679.36805555555</v>
+      </c>
+      <c r="F58" t="s">
+        <v>150</v>
+      </c>
+      <c r="G58" t="s">
+        <v>204</v>
+      </c>
+      <c r="H58" t="s">
+        <v>74</v>
+      </c>
+      <c r="I58" t="s">
+        <v>74</v>
+      </c>
+      <c r="J58" t="s">
+        <v>248</v>
+      </c>
+      <c r="K58" s="2">
+        <v>45680.83472222222</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59">
+        <v>9871440</v>
+      </c>
+      <c r="C59" t="s">
+        <v>76</v>
+      </c>
+      <c r="D59" t="s">
+        <v>92</v>
+      </c>
+      <c r="E59" s="2">
+        <v>45680.53125</v>
+      </c>
+      <c r="F59" t="s">
+        <v>151</v>
+      </c>
+      <c r="G59" t="s">
+        <v>205</v>
+      </c>
+      <c r="H59" t="s">
+        <v>74</v>
+      </c>
+      <c r="I59" t="s">
+        <v>74</v>
+      </c>
+      <c r="J59" t="s">
+        <v>248</v>
+      </c>
+      <c r="K59" s="2">
+        <v>45680.83472222222</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60">
+        <v>9563976</v>
+      </c>
+      <c r="C60" t="s">
+        <v>76</v>
+      </c>
+      <c r="D60" t="s">
+        <v>93</v>
+      </c>
+      <c r="E60" s="2">
+        <v>45680.46180555555</v>
+      </c>
+      <c r="F60" t="s">
+        <v>152</v>
+      </c>
+      <c r="G60" t="s">
+        <v>206</v>
+      </c>
+      <c r="H60" t="s">
+        <v>74</v>
+      </c>
+      <c r="I60" t="s">
+        <v>74</v>
+      </c>
+      <c r="J60" t="s">
+        <v>248</v>
+      </c>
+      <c r="K60" s="2">
+        <v>45680.66736111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>